<commit_message>
Update final analyses Excel sheet
</commit_message>
<xml_diff>
--- a/docs/Analyses_Edited.xlsx
+++ b/docs/Analyses_Edited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\musti\Desktop\Programs\Department of Energy\METIL Quickstart Internship\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8F73A3-6EDB-4FE4-8D0E-18C2EF54ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27252C5A-6EA4-404E-A2A0-9940E02925DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t>Feature</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Evaluation Time</t>
   </si>
   <si>
-    <t>Total without preprocessing</t>
-  </si>
-  <si>
     <t>Total Runtime</t>
   </si>
   <si>
@@ -187,14 +184,62 @@
   <si>
     <t>Runtime (%)</t>
   </si>
+  <si>
+    <t>Encryption Time</t>
+  </si>
+  <si>
+    <t>Decryption Time</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>All Others</t>
+  </si>
+  <si>
+    <t>Runtime Overhead</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Total Without Initial Preprocessing</t>
+  </si>
+  <si>
+    <t>Total Preprocessing Time</t>
+  </si>
+  <si>
+    <t>Additional Overhead Time</t>
+  </si>
+  <si>
+    <t>Inference only</t>
+  </si>
+  <si>
+    <t>Runtime w/o Pre (%)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Size (MB)</t>
+  </si>
+  <si>
+    <t>% Increase</t>
+  </si>
+  <si>
+    <t>Size Distribution (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000000000"/>
-    <numFmt numFmtId="166" formatCode="0.0000000000%"/>
+  <numFmts count="5">
+    <numFmt numFmtId="165" formatCode="0.0000000000%"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="169" formatCode="0.00000%"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -288,11 +333,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -302,27 +355,55 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +564,7 @@
             <c:numRef>
               <c:f>'Performance Metrics'!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.473499997637179</c:v>
@@ -573,7 +654,7 @@
             <c:numRef>
               <c:f>'Performance Metrics'!$C$3:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2.4735011171547998</c:v>
@@ -681,7 +762,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -877,17 +958,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Runtime Analysis'!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Plaintext Model</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -902,11 +972,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000004-ED3E-45B1-8873-AF34242EE204}"/>
-              </c:ext>
-            </c:extLst>
+            <c:extLst/>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -924,7 +990,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000002-ED3E-45B1-8873-AF34242EE204}"/>
+                <c16:uniqueId val="{00000004-ED3E-45B1-8873-AF34242EE204}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -944,77 +1010,31 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-ED3E-45B1-8873-AF34242EE204}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-ED3E-45B1-8873-AF34242EE204}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.2057556867891514"/>
-                  <c:y val="2.2369860017497814E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-ED3E-45B1-8873-AF34242EE204}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.7873687664041994E-2"/>
-                  <c:y val="0.68952974628171482"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-ED3E-45B1-8873-AF34242EE204}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.21006846019247583"/>
-                  <c:y val="0.68490048118985125"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-ED3E-45B1-8873-AF34242EE204}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1044,85 +1064,76 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="bestFit"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Runtime Analysis'!$A$4:$A$7</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Runtime Analysis'!$A$5:$A$7</c:f>
+              <c:f>('Runtime Analysis'!$A$5,'Runtime Analysis'!$A$14)</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Preprocessing Time</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Training Time</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Evaluation Time</c:v>
+                  <c:v>All Others</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'Runtime Analysis'!$D$4:$D$7</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Runtime Analysis'!$D$5:$D$7</c:f>
+              <c:f>('Runtime Analysis'!$D$5,'Runtime Analysis'!$D$14)</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.99945849878835868</c:v>
+                  <c:v>0.99657826712672481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4150121164123666E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.4217328732754071E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:categoryFilterExceptions/>
-            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-ED3E-45B1-8873-AF34242EE204}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="bestFit"/>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -1286,17 +1297,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Runtime Analysis'!$E$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Encrypted Inference</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -1377,95 +1377,37 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.34166666666666667"/>
-                  <c:y val="0.68518518518518501"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-5805-4AFD-9904-F4FABE888116}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-0.27777777777777779"/>
-                  <c:y val="0.56481481481481477"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-5805-4AFD-9904-F4FABE888116}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.2222222222222215E-2"/>
-                  <c:y val="0.32870370370370372"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000002-5805-4AFD-9904-F4FABE888116}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.5083333333333333"/>
-                  <c:y val="0.11111111111111094"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:dLblPos val="bestFit"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-5805-4AFD-9904-F4FABE888116}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1509,9 +1451,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Runtime Analysis'!$A$4:$A$7</c:f>
+              <c:f>'Runtime Analysis'!$A$4:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Context Setup Time</c:v>
                 </c:pt>
@@ -1522,6 +1464,12 @@
                   <c:v>Training Time</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Encryption Time</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Decryption Time</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>Evaluation Time</c:v>
                 </c:pt>
               </c:strCache>
@@ -1529,21 +1477,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Runtime Analysis'!$E$4:$E$7</c:f>
+              <c:f>'Runtime Analysis'!$E$4:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9401496907272244E-2</c:v>
+                  <c:v>1.6993306795332813E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19635715230801123</c:v>
+                  <c:v>0.17153579055536033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0196793987545025E-5</c:v>
+                  <c:v>5.7232979078077788E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61767331354216359</c:v>
+                  <c:v>0.19727910388346284</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.920642083007886E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5844130481449844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,7 +1542,7 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr rtl="0">
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
@@ -1605,6 +1559,741 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Encrypted Inference Runtime Distribution</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(Unique</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Stages Only)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Runtime Analysis'!$A$4,'Runtime Analysis'!$A$7:$A$9)</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Context Setup Time</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Encryption Time</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Decryption Time</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Evaluation Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Runtime Analysis'!$G$4,'Runtime Analysis'!$G$7:$G$9)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.052599767307503E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2382909033555749</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5278061722612927E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.70590503724873754</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8F93-4CC6-B54D-CB0C7025EB2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory Usage Increase (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D740-4158-9496-6A97D84DAA3B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Memory Usage'!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Coefficients</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Intercept</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Features</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Memory Usage'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1988.4047619047619</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7355.03125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1989.0466344997594</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1990.3344089571951</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D740-4158-9496-6A97D84DAA3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="983214352"/>
+        <c:axId val="983214832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="983214352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="983214832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="983214832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="983214352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1769,6 +2458,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3278,6 +4047,1028 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -3355,16 +5146,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3391,16 +5182,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>376237</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>71437</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3420,6 +5211,379 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9130972C-8734-F6C0-F0CC-10FCFB6E85A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19049" y="3086099"/>
+          <a:ext cx="11182351" cy="3457576"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200"/>
+            <a:t>Preprocessing Time:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Initial preprocessing + feature selection for both</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>Additional Overhead Time:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Inferencing - decryption + encryption + context setup</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Total Preprocessing Time</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Plaintext - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Initial preprocessing + feature selection only</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>	Inferencing - Initial preprocessing + </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>feature selection + decryption + encryption + context setup</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200"/>
+            <a:t>Training Time:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Plaintext model training time for both</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200"/>
+            <a:t>Evaluation Time:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Plaintext - evaluation step</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Inferencing - inferencing step</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200"/>
+            <a:t>Total Without Initial Preprocessing:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Plaintext - Only evaluation and training steps</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Inferencing - inferencing step + </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>decryption + encryption + context setup</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200"/>
+            <a:t>Total Runtime:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Plaintext - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>initial preprocessing + feature selection</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t> + training + evaluation</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" kern="1200" baseline="0"/>
+            <a:t>	Inferencing - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Inferencing - initial preprocessing + feature selection + plaintext training step + inferencing step + decryption + encryption + context setup</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33C203B2-4A64-888F-72A9-15D9558148EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C4E87CD-17E5-0BAF-6CCC-7F682DCDB252}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3716,7 +5880,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3724,18 +5888,18 @@
     <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3747,11 +5911,11 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>47</v>
+      <c r="D2" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3764,13 +5928,13 @@
       <c r="C3">
         <v>-17854.327049063719</v>
       </c>
-      <c r="D3" s="6">
-        <f>ABS(B3-C3)</f>
+      <c r="D3" s="29">
+        <f t="shared" ref="D3:D22" si="0">ABS(B3-C3)</f>
         <v>1.3606040738523006E-9</v>
       </c>
-      <c r="E3" s="13">
-        <f>D3/B3</f>
-        <v>-7.6205844673577153E-14</v>
+      <c r="E3" s="5">
+        <f>ABS(D3/B3)</f>
+        <v>7.6205844673577153E-14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3783,12 +5947,12 @@
       <c r="C4">
         <v>14042.59545713286</v>
       </c>
-      <c r="D4" s="6">
-        <f>ABS(B4-C4)</f>
+      <c r="D4" s="29">
+        <f t="shared" si="0"/>
         <v>1.9099388737231493E-10</v>
       </c>
-      <c r="E4" s="13">
-        <f t="shared" ref="E4:E22" si="0">D4/B4</f>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E22" si="1">ABS(D4/B4)</f>
         <v>1.3601038921569389E-14</v>
       </c>
     </row>
@@ -3802,12 +5966,12 @@
       <c r="C5">
         <v>5513.8770388193534</v>
       </c>
-      <c r="D5" s="6">
-        <f>ABS(B5-C5)</f>
+      <c r="D5" s="29">
+        <f t="shared" si="0"/>
         <v>1.0231815394945443E-9</v>
       </c>
-      <c r="E5" s="13">
-        <f t="shared" si="0"/>
+      <c r="E5" s="5">
+        <f t="shared" si="1"/>
         <v>1.8556480898845739E-13</v>
       </c>
     </row>
@@ -3821,12 +5985,12 @@
       <c r="C6">
         <v>4701.1175489331308</v>
       </c>
-      <c r="D6" s="6">
-        <f>ABS(B6-C6)</f>
+      <c r="D6" s="29">
+        <f t="shared" si="0"/>
         <v>3.8926373235881329E-10</v>
       </c>
-      <c r="E6" s="13">
-        <f t="shared" si="0"/>
+      <c r="E6" s="5">
+        <f t="shared" si="1"/>
         <v>8.2802382264855377E-14</v>
       </c>
     </row>
@@ -3840,12 +6004,12 @@
       <c r="C7">
         <v>4363.9402459384264</v>
       </c>
-      <c r="D7" s="6">
-        <f>ABS(B7-C7)</f>
+      <c r="D7" s="29">
+        <f t="shared" si="0"/>
         <v>1.9281287677586079E-10</v>
       </c>
-      <c r="E7" s="13">
-        <f t="shared" si="0"/>
+      <c r="E7" s="5">
+        <f t="shared" si="1"/>
         <v>4.4183207356086661E-14</v>
       </c>
     </row>
@@ -3859,13 +6023,13 @@
       <c r="C8">
         <v>-4350.7255227994428</v>
       </c>
-      <c r="D8" s="6">
-        <f>ABS(B8-C8)</f>
+      <c r="D8" s="29">
+        <f t="shared" si="0"/>
         <v>2.6375346351414919E-10</v>
       </c>
-      <c r="E8" s="13">
-        <f t="shared" si="0"/>
-        <v>-6.062286902080252E-14</v>
+      <c r="E8" s="5">
+        <f t="shared" si="1"/>
+        <v>6.062286902080252E-14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,13 +6042,13 @@
       <c r="C9">
         <v>-2201.59933892755</v>
       </c>
-      <c r="D9" s="6">
-        <f>ABS(B9-C9)</f>
+      <c r="D9" s="29">
+        <f t="shared" si="0"/>
         <v>2.5102053768932819E-10</v>
       </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>-1.1401735695086895E-13</v>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>1.1401735695086895E-13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3897,13 +6061,13 @@
       <c r="C10">
         <v>-1364.8223364273449</v>
       </c>
-      <c r="D10" s="6">
-        <f>ABS(B10-C10)</f>
+      <c r="D10" s="29">
+        <f t="shared" si="0"/>
         <v>1.3660610420629382E-9</v>
       </c>
-      <c r="E10" s="13">
-        <f t="shared" si="0"/>
-        <v>-1.0009075947844381E-12</v>
+      <c r="E10" s="5">
+        <f t="shared" si="1"/>
+        <v>1.0009075947844381E-12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3916,13 +6080,13 @@
       <c r="C11">
         <v>-427.66147859336411</v>
       </c>
-      <c r="D11" s="6">
-        <f>ABS(B11-C11)</f>
+      <c r="D11" s="29">
+        <f t="shared" si="0"/>
         <v>3.2327989174518734E-9</v>
       </c>
-      <c r="E11" s="13">
-        <f t="shared" si="0"/>
-        <v>-7.5592473936641304E-12</v>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5592473936641304E-12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3935,13 +6099,13 @@
       <c r="C12">
         <v>-321.23336876825408</v>
       </c>
-      <c r="D12" s="6">
-        <f>ABS(B12-C12)</f>
+      <c r="D12" s="29">
+        <f t="shared" si="0"/>
         <v>8.4503426478477195E-10</v>
       </c>
-      <c r="E12" s="13">
-        <f t="shared" si="0"/>
-        <v>-2.6305930421324886E-12</v>
+      <c r="E12" s="5">
+        <f t="shared" si="1"/>
+        <v>2.6305930421324886E-12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3954,13 +6118,13 @@
       <c r="C13">
         <v>-201.7694550917827</v>
       </c>
-      <c r="D13" s="6">
-        <f>ABS(B13-C13)</f>
+      <c r="D13" s="29">
+        <f t="shared" si="0"/>
         <v>1.3885994576412486E-9</v>
       </c>
-      <c r="E13" s="13">
-        <f t="shared" si="0"/>
-        <v>-6.8821093709112043E-12</v>
+      <c r="E13" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8821093709112043E-12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3973,12 +6137,12 @@
       <c r="C14">
         <v>201.26295436397751</v>
       </c>
-      <c r="D14" s="6">
-        <f>ABS(B14-C14)</f>
+      <c r="D14" s="29">
+        <f t="shared" si="0"/>
         <v>5.7301008382637519E-10</v>
       </c>
-      <c r="E14" s="13">
-        <f t="shared" si="0"/>
+      <c r="E14" s="5">
+        <f t="shared" si="1"/>
         <v>2.8470718103031345E-12</v>
       </c>
     </row>
@@ -3992,12 +6156,12 @@
       <c r="C15">
         <v>185.07187106653009</v>
       </c>
-      <c r="D15" s="6">
-        <f>ABS(B15-C15)</f>
+      <c r="D15" s="29">
+        <f t="shared" si="0"/>
         <v>1.5726868696219753E-9</v>
       </c>
-      <c r="E15" s="13">
-        <f t="shared" si="0"/>
+      <c r="E15" s="5">
+        <f t="shared" si="1"/>
         <v>8.4977088121078452E-12</v>
       </c>
     </row>
@@ -4011,12 +6175,12 @@
       <c r="C16">
         <v>151.56010827042971</v>
       </c>
-      <c r="D16" s="6">
-        <f>ABS(B16-C16)</f>
+      <c r="D16" s="29">
+        <f t="shared" si="0"/>
         <v>4.4778403207601514E-10</v>
       </c>
-      <c r="E16" s="13">
-        <f t="shared" si="0"/>
+      <c r="E16" s="5">
+        <f t="shared" si="1"/>
         <v>2.954497969054681E-12</v>
       </c>
     </row>
@@ -4030,12 +6194,12 @@
       <c r="C17">
         <v>143.01838576810829</v>
       </c>
-      <c r="D17" s="6">
-        <f>ABS(B17-C17)</f>
+      <c r="D17" s="29">
+        <f t="shared" si="0"/>
         <v>8.6998852566466667E-11</v>
       </c>
-      <c r="E17" s="13">
-        <f t="shared" si="0"/>
+      <c r="E17" s="5">
+        <f t="shared" si="1"/>
         <v>6.0830537346068717E-13</v>
       </c>
     </row>
@@ -4049,12 +6213,12 @@
       <c r="C18">
         <v>114.7607661656252</v>
       </c>
-      <c r="D18" s="6">
-        <f>ABS(B18-C18)</f>
+      <c r="D18" s="29">
+        <f t="shared" si="0"/>
         <v>3.1604940886609256E-11</v>
       </c>
-      <c r="E18" s="13">
-        <f t="shared" si="0"/>
+      <c r="E18" s="5">
+        <f t="shared" si="1"/>
         <v>2.7539848279685612E-13</v>
       </c>
     </row>
@@ -4068,12 +6232,12 @@
       <c r="C19">
         <v>10.597376279514719</v>
       </c>
-      <c r="D19" s="6">
-        <f>ABS(B19-C19)</f>
+      <c r="D19" s="29">
+        <f t="shared" si="0"/>
         <v>2.6645796680213607E-9</v>
       </c>
-      <c r="E19" s="13">
-        <f t="shared" si="0"/>
+      <c r="E19" s="5">
+        <f t="shared" si="1"/>
         <v>2.5143767637109917E-10</v>
       </c>
     </row>
@@ -4087,13 +6251,13 @@
       <c r="C20">
         <v>-7.0894858673927956</v>
       </c>
-      <c r="D20" s="6">
-        <f>ABS(B20-C20)</f>
+      <c r="D20" s="29">
+        <f t="shared" si="0"/>
         <v>2.1650947701346013E-10</v>
       </c>
-      <c r="E20" s="13">
-        <f t="shared" si="0"/>
-        <v>-3.0539517402225243E-11</v>
+      <c r="E20" s="5">
+        <f t="shared" si="1"/>
+        <v>3.0539517402225243E-11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -4106,12 +6270,12 @@
       <c r="C21">
         <v>6.2096842348569226</v>
       </c>
-      <c r="D21" s="6">
-        <f>ABS(B21-C21)</f>
+      <c r="D21" s="29">
+        <f t="shared" si="0"/>
         <v>9.9900621108872656E-10</v>
       </c>
-      <c r="E21" s="13">
-        <f t="shared" si="0"/>
+      <c r="E21" s="5">
+        <f t="shared" si="1"/>
         <v>1.6087874570501825E-10</v>
       </c>
     </row>
@@ -4125,13 +6289,13 @@
       <c r="C22">
         <v>-0.29261681705247611</v>
       </c>
-      <c r="D22" s="6">
-        <f>ABS(B22-C22)</f>
+      <c r="D22" s="29">
+        <f t="shared" si="0"/>
         <v>6.4288052659122741E-10</v>
       </c>
-      <c r="E22" s="13">
-        <f t="shared" si="0"/>
-        <v>-2.1970047192754089E-9</v>
+      <c r="E22" s="5">
+        <f t="shared" si="1"/>
+        <v>2.1970047192754089E-9</v>
       </c>
     </row>
   </sheetData>
@@ -4147,58 +6311,59 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>47</v>
+      <c r="D2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <v>2.473499997637179</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <v>2.4735011171547998</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="14">
         <f>ABS(B3-C3)</f>
         <v>1.1195176208289581E-6</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="16">
         <f>D3/B3</f>
         <v>4.5260465813559004E-7</v>
       </c>
@@ -4207,17 +6372,17 @@
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="12">
         <v>15.027666515264521</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="12">
         <v>15.0277092978497</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="14">
         <f t="shared" ref="D4:D6" si="0">ABS(B4-C4)</f>
         <v>4.2782585179423904E-5</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="16">
         <f t="shared" ref="E4:E6" si="1">D4/B4</f>
         <v>2.8469213856966424E-6</v>
       </c>
@@ -4226,17 +6391,17 @@
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="12">
         <v>3.8765534325305668</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="12">
         <v>3.8765589506480742</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="14">
         <f t="shared" si="0"/>
         <v>5.5181175073748534E-6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="16">
         <f t="shared" si="1"/>
         <v>1.4234596796909603E-6</v>
       </c>
@@ -4245,17 +6410,17 @@
       <c r="A6" t="s">
         <v>29</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="12">
         <v>0.92638931265907243</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>0.92638910309523237</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="14">
         <f t="shared" si="0"/>
         <v>2.0956384005899054E-7</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="16">
         <f t="shared" si="1"/>
         <v>2.2621573586321555E-7</v>
       </c>
@@ -4271,171 +6436,339 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P26" sqref="P26"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" s="10"/>
+      <c r="F2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
-      <c r="C4">
-        <v>0.41945409774780268</v>
-      </c>
-      <c r="D4" s="8">
-        <f>B4/$B$9</f>
+      <c r="C4" s="20">
+        <v>0.410871982574463</v>
+      </c>
+      <c r="D4" s="2">
+        <f>B4/B$13</f>
         <v>0</v>
       </c>
-      <c r="E4" s="8">
-        <f>C4/$C$9</f>
-        <v>1.9401496907272244E-2</v>
+      <c r="E4" s="2">
+        <f>C4/C$13</f>
+        <v>1.6993306795332813E-2</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="2">
+        <f>C4/$C$12</f>
+        <v>2.052599767307503E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
-      <c r="B5">
-        <v>3.599197149276733</v>
-      </c>
-      <c r="C5">
-        <v>4.24517822265625</v>
-      </c>
-      <c r="D5" s="8">
-        <f t="shared" ref="D5:D9" si="0">B5/$B$9</f>
-        <v>0.99945849878835868</v>
-      </c>
-      <c r="E5" s="8">
-        <f t="shared" ref="E5:E9" si="1">C5/$C$9</f>
-        <v>0.19635715230801123</v>
+      <c r="B5" s="20">
+        <v>4.1474711894989014</v>
+      </c>
+      <c r="C5" s="20">
+        <v>4.1474711894989014</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" ref="D5:D13" si="0">B5/B$13</f>
+        <v>0.99657826712672481</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E13" si="1">C5/C$13</f>
+        <v>0.17153579055536033</v>
+      </c>
+      <c r="F5" s="20">
+        <f>C5/B5</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="B6">
-        <v>1.9500255584716799E-3</v>
-      </c>
-      <c r="C6">
-        <v>1.9500255584716799E-3</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="B6" s="20">
+        <v>1.3838052749633791E-2</v>
+      </c>
+      <c r="C6" s="20">
+        <v>1.3838052749633791E-2</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>5.4150121164123666E-4</v>
-      </c>
-      <c r="E6" s="8">
+        <v>3.3250870227996567E-3</v>
+      </c>
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>9.0196793987545025E-5</v>
+        <v>5.7232979078077788E-4</v>
+      </c>
+      <c r="F6" s="20">
+        <f>C6/B6</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>13.353897571563721</v>
-      </c>
-      <c r="D7" s="8">
+        <v>49</v>
+      </c>
+      <c r="C7" s="20">
+        <v>4.7699048519134521</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>0.61767331354216359</v>
+        <v>0.19727910388346284</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="2">
+        <f>C7/$C$12</f>
+        <v>0.2382909033555749</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="20">
+        <v>0.70616626739501953</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.920642083007886E-2</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" ref="G8:G9" si="2">C8/$C$12</f>
+        <v>3.5278061722612927E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="20">
+        <v>4.0221214294433588E-4</v>
+      </c>
+      <c r="C9" s="20">
+        <v>14.130207300186161</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>9.664585047575023E-5</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5844130481449844</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.70590503724873754</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="20">
+        <v>5.8869431018829346</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.24347883150887453</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="2">
+        <f>SUM(G4,G7,G8)</f>
+        <v>0.2940949627512629</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="20">
+        <f>B5</f>
+        <v>4.1474711894989014</v>
+      </c>
+      <c r="C11" s="20">
+        <f>C10+C5</f>
+        <v>10.034414291381836</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99657826712672481</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.41501462206423484</v>
+      </c>
+      <c r="F11" s="20">
+        <f>C11/B11</f>
+        <v>2.4194054239094536</v>
+      </c>
+      <c r="G11" s="2">
+        <f>SUM(G4,G7,G8)</f>
+        <v>0.2940949627512629</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="20">
+        <v>1.424026489257812E-2</v>
+      </c>
+      <c r="C12" s="20">
+        <v>20.017150402069088</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4217328732754054E-3</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.82789187965385858</v>
+      </c>
+      <c r="F12" s="20">
+        <f>C12/B12</f>
+        <v>1405.6726158585591</v>
+      </c>
+      <c r="G12" s="2">
+        <f>SUM(G4,G7,G8)</f>
+        <v>0.2940949627512629</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>35</v>
       </c>
-      <c r="B8">
-        <v>1.9500255584716799E-3</v>
-      </c>
-      <c r="C8">
-        <v>18.01852989196777</v>
-      </c>
-      <c r="D8" s="8">
-        <f t="shared" si="0"/>
-        <v>5.4150121164123666E-4</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="1"/>
-        <v>0.83343196275744691</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9">
-        <v>3.6011471748352051</v>
-      </c>
-      <c r="C9">
-        <v>21.619677066802979</v>
-      </c>
-      <c r="D9" s="8">
+      <c r="B13" s="20">
+        <v>4.1617114543914786</v>
+      </c>
+      <c r="C13" s="20">
+        <v>24.178459644317631</v>
+      </c>
+      <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E13" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="F13" s="20">
+        <f>C13/B13</f>
+        <v>5.8097395528957883</v>
+      </c>
+      <c r="G13" s="2">
+        <f>SUM(G4,G7:G9)</f>
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="2">
+        <f>D6 + D9</f>
+        <v>3.4217328732754071E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -4444,81 +6777,336 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+      <c r="B2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="10"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="4"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="20">
+        <v>0.1640625</v>
+      </c>
+      <c r="C4" s="20">
+        <v>326.38671875</v>
+      </c>
+      <c r="D4" s="27">
+        <f>(C4-B4)/B4</f>
+        <v>1988.4047619047619</v>
+      </c>
+      <c r="E4" s="2">
+        <f>B4/B$7</f>
+        <v>1.2607312241099838E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <f>C4/C$7</f>
+        <v>1.2595095476906082E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="20">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C5" s="20">
+        <v>229.8759765625</v>
+      </c>
+      <c r="D5" s="27">
+        <f t="shared" ref="D5:D7" si="0">(C5-B5)/B5</f>
+        <v>7355.03125</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E7" si="1">B5/B$7</f>
+        <v>2.4013928078285405E-4</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F7" si="2">C5/C$7</f>
+        <v>8.8707956124569243E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="20">
+        <v>129.9375</v>
+      </c>
+      <c r="C6" s="20">
+        <v>258581.6845703125</v>
+      </c>
+      <c r="D6" s="27">
+        <f t="shared" si="0"/>
+        <v>1989.0466344997594</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>0.99849912949510711</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.99785341089106372</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="20">
+        <f>SUM(B4:B6)</f>
+        <v>130.1328125</v>
+      </c>
+      <c r="C7" s="20">
+        <f>SUM(C4:C6)</f>
+        <v>259137.947265625</v>
+      </c>
+      <c r="D7" s="27">
+        <f t="shared" si="0"/>
+        <v>1990.3344089571951</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <f>C7/C$7</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="2">
+        <f>SUM(E4:E5)</f>
+        <v>1.5008705048928379E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <f>SUM(F4:F5)</f>
+        <v>2.1465891089363005E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C11" s="19" t="s">
         <v>25</v>
       </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="20">
+        <f>B4/1024</f>
+        <v>1.6021728515625E-4</v>
+      </c>
+      <c r="C12" s="20">
+        <f>C4/1024</f>
+        <v>0.31873703002929688</v>
+      </c>
+      <c r="D12" s="27">
+        <f>(C12-B12)/B12</f>
+        <v>1988.4047619047619</v>
+      </c>
+      <c r="E12" s="2">
+        <f>B12/B$15</f>
+        <v>1.2607312241099838E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <f>C12/C$15</f>
+        <v>1.2595095476906082E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B4">
-        <v>0.1640625</v>
-      </c>
-      <c r="C4">
-        <v>326.38671875</v>
+      <c r="B13" s="20">
+        <f t="shared" ref="B13:C13" si="3">B5/1024</f>
+        <v>3.0517578125E-5</v>
+      </c>
+      <c r="C13" s="20">
+        <f t="shared" si="3"/>
+        <v>0.22448825836181641</v>
+      </c>
+      <c r="D13" s="27">
+        <f t="shared" ref="D13:D15" si="4">(C13-B13)/B13</f>
+        <v>7355.03125</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" ref="E13:E15" si="5">B13/B$15</f>
+        <v>2.4013928078285405E-4</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" ref="F13:F15" si="6">C13/C$15</f>
+        <v>8.8707956124569243E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B5">
-        <v>3.125E-2</v>
-      </c>
-      <c r="C5">
-        <v>229.8759765625</v>
+      <c r="B14" s="20">
+        <f t="shared" ref="B14:C14" si="7">B6/1024</f>
+        <v>0.12689208984375</v>
+      </c>
+      <c r="C14" s="20">
+        <f t="shared" si="7"/>
+        <v>252.5211763381958</v>
+      </c>
+      <c r="D14" s="27">
+        <f t="shared" si="4"/>
+        <v>1989.0466344997594</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="5"/>
+        <v>0.99849912949510711</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="6"/>
+        <v>0.99785341089106372</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6">
-        <v>129.9375</v>
-      </c>
-      <c r="C6">
-        <v>258581.6845703125</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="20">
+        <f>SUM(B12:B14)</f>
+        <v>0.12708282470703125</v>
+      </c>
+      <c r="C15" s="20">
+        <f>SUM(C12:C14)</f>
+        <v>253.06440162658691</v>
+      </c>
+      <c r="D15" s="27">
+        <f t="shared" si="4"/>
+        <v>1990.3344089571951</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="2">
+        <f>SUM(E12:E13)</f>
+        <v>1.5008705048928379E-3</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(F12:F13)</f>
+        <v>2.1465891089363005E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
+  <mergeCells count="6">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="A9:F9"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>